<commit_message>
separated opening excel file from extracting dataframe
</commit_message>
<xml_diff>
--- a/Sample Roster 24.xlsx
+++ b/Sample Roster 24.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Roster" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="01" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Unit 1 Groups" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet6" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -375,7 +375,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.05"/>
@@ -611,7 +611,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.78"/>
@@ -748,7 +748,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.46"/>
@@ -790,7 +790,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.944463306379377</v>
+        <v>0.201222836636421</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -807,7 +807,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.366391644106837</v>
+        <v>0.200249621758525</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>59</v>
@@ -819,7 +819,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.821518948407731</v>
+        <v>0.541780045080492</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>51</v>
@@ -831,7 +831,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0936192888590535</v>
+        <v>0.639918177869707</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>46</v>
@@ -843,7 +843,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.0589086930425</v>
+        <v>0.274778704311162</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>44</v>
@@ -855,13 +855,13 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.322399136848558</v>
+        <v>0.586190868254914</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.966831861369946</v>
+        <v>0.772186833056835</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>34</v>
@@ -878,7 +878,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.34151930224098</v>
+        <v>0.183272022594158</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>50</v>
@@ -893,7 +893,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.921373139105808</v>
+        <v>0.590021716410087</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>56</v>
@@ -908,7 +908,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.626024812856966</v>
+        <v>0.695844712703128</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>40</v>
@@ -923,7 +923,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.991052260493384</v>
+        <v>0.759757608682902</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>65</v>
@@ -938,7 +938,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.547762208462025</v>
+        <v>0.321940900423674</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>66</v>
@@ -947,55 +947,55 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.613539097685592</v>
+        <v>0.617939689411237</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.884472548879852</v>
+        <v>0.22100026549909</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.582922444720995</v>
+        <v>0.300779479027105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.825597017083178</v>
+        <v>0.729878083929235</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.142826017583424</v>
+        <v>0.721828340565894</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.215464320129282</v>
+        <v>0.0471569385374919</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.184818944462692</v>
+        <v>0.549716383331881</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.903514319697025</v>
+        <v>0.296734774002345</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.225132550908772</v>
+        <v>0.86827155962695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>